<commit_message>
Deploying to gh-pages from  @ b36d5d9b073e2a34da1353465f4ef9aedf86ce5e 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/1.3.1.xlsx
+++ b/en/downloads/data-excel/1.3.1.xlsx
@@ -375,7 +375,7 @@
     <xf numFmtId="166" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -460,6 +460,9 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="22">
     <cellStyle name="Normal 17" xfId="3"/>
@@ -8138,9 +8141,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q22"/>
+  <dimension ref="A1:R22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R24" sqref="R24:R25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -8148,7 +8153,7 @@
     <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="39" customHeight="1">
+    <row r="1" spans="1:18" ht="39" customHeight="1">
       <c r="A1" s="18" t="s">
         <v>15</v>
       </c>
@@ -8172,7 +8177,7 @@
       <c r="O1" s="22"/>
       <c r="P1" s="23"/>
     </row>
-    <row r="2" spans="1:17" ht="15.75" thickBot="1">
+    <row r="2" spans="1:18" ht="15.75" thickBot="1">
       <c r="A2" s="20"/>
       <c r="B2" s="21"/>
       <c r="C2" s="21"/>
@@ -8190,8 +8195,9 @@
       <c r="O2" s="24"/>
       <c r="P2" s="24"/>
       <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
     </row>
-    <row r="3" spans="1:17" ht="15.75" thickBot="1">
+    <row r="3" spans="1:18" ht="15.75" thickBot="1">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -8243,8 +8249,11 @@
       <c r="Q3" s="5">
         <v>2020</v>
       </c>
+      <c r="R3" s="5">
+        <v>2021</v>
+      </c>
     </row>
-    <row r="4" spans="1:17" s="30" customFormat="1" ht="27" customHeight="1">
+    <row r="4" spans="1:18" s="30" customFormat="1" ht="27" customHeight="1">
       <c r="A4" s="29" t="s">
         <v>16</v>
       </c>
@@ -8296,8 +8305,11 @@
       <c r="Q4" s="27">
         <v>17.7</v>
       </c>
+      <c r="R4" s="32">
+        <v>18</v>
+      </c>
     </row>
-    <row r="5" spans="1:17" s="2" customFormat="1">
+    <row r="5" spans="1:18" s="2" customFormat="1">
       <c r="A5" s="22" t="s">
         <v>18</v>
       </c>
@@ -8349,8 +8361,11 @@
       <c r="Q5" s="25">
         <v>1.7006983633535606</v>
       </c>
+      <c r="R5" s="25">
+        <v>1.7480265877296817</v>
+      </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:18">
       <c r="A6" s="22" t="s">
         <v>19</v>
       </c>
@@ -8402,8 +8417,11 @@
       <c r="Q6" s="28">
         <v>4.0792532187560786</v>
       </c>
+      <c r="R6" s="25">
+        <v>4.1112601249414027</v>
+      </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:18">
       <c r="A7" s="22" t="s">
         <v>20</v>
       </c>
@@ -8455,8 +8473,11 @@
       <c r="Q7" s="28">
         <v>1.4965639329659175</v>
       </c>
+      <c r="R7" s="25">
+        <v>1.5225742120245318</v>
+      </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:18">
       <c r="A8" s="22" t="s">
         <v>21</v>
       </c>
@@ -8508,8 +8529,11 @@
       <c r="Q8" s="28">
         <v>1.2345401844834025</v>
       </c>
+      <c r="R8" s="25">
+        <v>1.2326518235454269</v>
+      </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:18">
       <c r="A9" s="22" t="s">
         <v>22</v>
       </c>
@@ -8561,8 +8585,11 @@
       <c r="Q9" s="28">
         <v>3.9182419607753913</v>
       </c>
+      <c r="R9" s="25">
+        <v>4.0865392096984241</v>
+      </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:18">
       <c r="A10" s="22" t="s">
         <v>23</v>
       </c>
@@ -8614,8 +8641,11 @@
       <c r="Q10" s="28">
         <v>0.84723021008759791</v>
       </c>
+      <c r="R10" s="25">
+        <v>0.84876624403485645</v>
+      </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:18">
       <c r="A11" s="22" t="s">
         <v>24</v>
       </c>
@@ -8667,8 +8697,11 @@
       <c r="Q11" s="28">
         <v>2.085763280904978</v>
       </c>
+      <c r="R11" s="25">
+        <v>2.1456657699653627</v>
+      </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:18">
       <c r="A12" s="22" t="s">
         <v>25</v>
       </c>
@@ -8720,8 +8753,11 @@
       <c r="Q12" s="28">
         <v>1.8003095767645958</v>
       </c>
+      <c r="R12" s="25">
+        <v>1.8214779402142154</v>
+      </c>
     </row>
-    <row r="13" spans="1:17" ht="15.75" thickBot="1">
+    <row r="13" spans="1:18" ht="15.75" thickBot="1">
       <c r="A13" s="24" t="s">
         <v>26</v>
       </c>
@@ -8773,8 +8809,11 @@
       <c r="Q13" s="26">
         <v>0.49216467627561039</v>
       </c>
+      <c r="R13" s="26">
+        <v>0.51989507542472779</v>
+      </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:18">
       <c r="A14" s="9"/>
       <c r="B14" s="12"/>
       <c r="C14" s="10"/>
@@ -8792,7 +8831,7 @@
       <c r="O14" s="23"/>
       <c r="P14" s="23"/>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:18">
       <c r="A15" s="9"/>
       <c r="B15" s="12"/>
       <c r="C15" s="10"/>
@@ -8810,7 +8849,7 @@
       <c r="O15" s="6"/>
       <c r="P15" s="6"/>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:18">
       <c r="A16" s="9"/>
       <c r="B16" s="12"/>
       <c r="C16" s="10"/>

</xml_diff>